<commit_message>
Update spreadsheet to include penstock material roughness value and Miller table
</commit_message>
<xml_diff>
--- a/Spreadsheet Interface/Input_Spreadsheet_v250123.xlsx
+++ b/Spreadsheet Interface/Input_Spreadsheet_v250123.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://kleinschmidtgroup-my.sharepoint.com/personal/kevin_nebiolo_kleinschmidtgroup_com/Documents/Software/stryke/Spreadsheet Interface/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://kleinschmidtgroup-my.sharepoint.com/personal/andrew_yoder_kleinschmidtgroup_com/Documents/Software/stryke/Spreadsheet Interface/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A6B91651-D364-4E5F-AC61-FFEA3897CD02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="11" documentId="8_{A6B91651-D364-4E5F-AC61-FFEA3897CD02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CAA4A503-2E57-44C5-97CA-0080D1D6F6D7}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Flow Scenarios" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="110">
   <si>
     <t>Scenario Number</t>
   </si>
@@ -368,6 +368,9 @@
   <si>
     <t xml:space="preserve">This sheet contains information that describe facility discharge.  The end user can either pass a stable discharge into the flow column, or type 'hydrograph'.  If the End User is in the United States and would like to fetch data from a particular USGS Gage and discharge year, enter the gage ID into the Gage column.  If the end user is in Canada, or there is no Gage ID, they will leave the Gage column blank and either use a hard coded stable discharge, or import their own gage data into the Hydrology tab.  The prorate column increases or decreases discharge based on difference in watersheds.  </t>
   </si>
+  <si>
+    <t>roughness</t>
+  </si>
 </sst>
 </file>
 
@@ -599,11 +602,15 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -611,16 +618,12 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -938,7 +941,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AZ7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
@@ -966,36 +969,36 @@
       <c r="I1" s="4"/>
     </row>
     <row r="2" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="38" t="s">
+      <c r="B2" s="39" t="s">
         <v>108</v>
       </c>
-      <c r="C2" s="39"/>
-      <c r="D2" s="39"/>
-      <c r="E2" s="40"/>
-      <c r="F2" s="39"/>
-      <c r="G2" s="39"/>
-      <c r="H2" s="39"/>
-      <c r="I2" s="39"/>
+      <c r="C2" s="40"/>
+      <c r="D2" s="40"/>
+      <c r="E2" s="41"/>
+      <c r="F2" s="40"/>
+      <c r="G2" s="40"/>
+      <c r="H2" s="40"/>
+      <c r="I2" s="40"/>
     </row>
     <row r="3" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B3" s="39"/>
-      <c r="C3" s="39"/>
-      <c r="D3" s="39"/>
-      <c r="E3" s="40"/>
-      <c r="F3" s="39"/>
-      <c r="G3" s="39"/>
-      <c r="H3" s="39"/>
-      <c r="I3" s="39"/>
+      <c r="B3" s="40"/>
+      <c r="C3" s="40"/>
+      <c r="D3" s="40"/>
+      <c r="E3" s="41"/>
+      <c r="F3" s="40"/>
+      <c r="G3" s="40"/>
+      <c r="H3" s="40"/>
+      <c r="I3" s="40"/>
     </row>
     <row r="4" spans="2:9" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="39"/>
-      <c r="C4" s="39"/>
-      <c r="D4" s="39"/>
-      <c r="E4" s="40"/>
-      <c r="F4" s="39"/>
-      <c r="G4" s="39"/>
-      <c r="H4" s="39"/>
-      <c r="I4" s="39"/>
+      <c r="B4" s="40"/>
+      <c r="C4" s="40"/>
+      <c r="D4" s="40"/>
+      <c r="E4" s="41"/>
+      <c r="F4" s="40"/>
+      <c r="G4" s="40"/>
+      <c r="H4" s="40"/>
+      <c r="I4" s="40"/>
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B5" s="5"/>
@@ -1078,31 +1081,31 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="47"/>
+    <col min="1" max="1" width="9.140625" style="38"/>
     <col min="3" max="3" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="37" width="9.140625" style="47"/>
+    <col min="4" max="37" width="9.140625" style="38"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B1" s="47"/>
-      <c r="C1" s="47"/>
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
     </row>
     <row r="2" spans="2:10" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="44" t="s">
+      <c r="B2" s="42" t="s">
         <v>107</v>
       </c>
-      <c r="C2" s="44"/>
-      <c r="D2" s="44"/>
-      <c r="E2" s="44"/>
-      <c r="F2" s="44"/>
-      <c r="G2" s="44"/>
-      <c r="H2" s="44"/>
-      <c r="I2" s="44"/>
-      <c r="J2" s="44"/>
+      <c r="C2" s="42"/>
+      <c r="D2" s="42"/>
+      <c r="E2" s="42"/>
+      <c r="F2" s="42"/>
+      <c r="G2" s="42"/>
+      <c r="H2" s="42"/>
+      <c r="I2" s="42"/>
+      <c r="J2" s="42"/>
     </row>
     <row r="3" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B3" s="47"/>
-      <c r="C3" s="47"/>
+      <c r="B3" s="38"/>
+      <c r="C3" s="38"/>
     </row>
     <row r="4" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B4" s="37" t="s">
@@ -1111,10 +1114,10 @@
       <c r="C4" s="37" t="s">
         <v>105</v>
       </c>
-      <c r="E4" s="48" t="s">
+      <c r="E4" t="s">
         <v>106</v>
       </c>
-      <c r="F4" s="48"/>
+      <c r="F4"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1156,71 +1159,71 @@
       <c r="K1" s="29"/>
     </row>
     <row r="2" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B2" s="42" t="s">
+      <c r="B2" s="44" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="39"/>
-      <c r="D2" s="39"/>
-      <c r="E2" s="39"/>
-      <c r="F2" s="39"/>
-      <c r="G2" s="39"/>
-      <c r="H2" s="39"/>
-      <c r="I2" s="39"/>
-      <c r="J2" s="39"/>
-      <c r="K2" s="39"/>
-      <c r="L2" s="43"/>
+      <c r="C2" s="40"/>
+      <c r="D2" s="40"/>
+      <c r="E2" s="40"/>
+      <c r="F2" s="40"/>
+      <c r="G2" s="40"/>
+      <c r="H2" s="40"/>
+      <c r="I2" s="40"/>
+      <c r="J2" s="40"/>
+      <c r="K2" s="40"/>
+      <c r="L2" s="45"/>
     </row>
     <row r="3" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B3" s="39"/>
-      <c r="C3" s="39"/>
-      <c r="D3" s="39"/>
-      <c r="E3" s="39"/>
-      <c r="F3" s="39"/>
-      <c r="G3" s="39"/>
-      <c r="H3" s="39"/>
-      <c r="I3" s="39"/>
-      <c r="J3" s="39"/>
-      <c r="K3" s="39"/>
-      <c r="L3" s="43"/>
+      <c r="B3" s="40"/>
+      <c r="C3" s="40"/>
+      <c r="D3" s="40"/>
+      <c r="E3" s="40"/>
+      <c r="F3" s="40"/>
+      <c r="G3" s="40"/>
+      <c r="H3" s="40"/>
+      <c r="I3" s="40"/>
+      <c r="J3" s="40"/>
+      <c r="K3" s="40"/>
+      <c r="L3" s="45"/>
     </row>
     <row r="4" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B4" s="39"/>
-      <c r="C4" s="39"/>
-      <c r="D4" s="39"/>
-      <c r="E4" s="39"/>
-      <c r="F4" s="39"/>
-      <c r="G4" s="39"/>
-      <c r="H4" s="39"/>
-      <c r="I4" s="39"/>
-      <c r="J4" s="39"/>
-      <c r="K4" s="39"/>
-      <c r="L4" s="43"/>
+      <c r="B4" s="40"/>
+      <c r="C4" s="40"/>
+      <c r="D4" s="40"/>
+      <c r="E4" s="40"/>
+      <c r="F4" s="40"/>
+      <c r="G4" s="40"/>
+      <c r="H4" s="40"/>
+      <c r="I4" s="40"/>
+      <c r="J4" s="40"/>
+      <c r="K4" s="40"/>
+      <c r="L4" s="45"/>
     </row>
     <row r="5" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B5" s="39"/>
-      <c r="C5" s="39"/>
-      <c r="D5" s="39"/>
-      <c r="E5" s="39"/>
-      <c r="F5" s="39"/>
-      <c r="G5" s="39"/>
-      <c r="H5" s="39"/>
-      <c r="I5" s="39"/>
-      <c r="J5" s="39"/>
-      <c r="K5" s="39"/>
-      <c r="L5" s="43"/>
+      <c r="B5" s="40"/>
+      <c r="C5" s="40"/>
+      <c r="D5" s="40"/>
+      <c r="E5" s="40"/>
+      <c r="F5" s="40"/>
+      <c r="G5" s="40"/>
+      <c r="H5" s="40"/>
+      <c r="I5" s="40"/>
+      <c r="J5" s="40"/>
+      <c r="K5" s="40"/>
+      <c r="L5" s="45"/>
     </row>
     <row r="6" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B6" s="39"/>
-      <c r="C6" s="39"/>
-      <c r="D6" s="39"/>
-      <c r="E6" s="39"/>
-      <c r="F6" s="39"/>
-      <c r="G6" s="39"/>
-      <c r="H6" s="39"/>
-      <c r="I6" s="39"/>
-      <c r="J6" s="39"/>
-      <c r="K6" s="39"/>
-      <c r="L6" s="43"/>
+      <c r="B6" s="40"/>
+      <c r="C6" s="40"/>
+      <c r="D6" s="40"/>
+      <c r="E6" s="40"/>
+      <c r="F6" s="40"/>
+      <c r="G6" s="40"/>
+      <c r="H6" s="40"/>
+      <c r="I6" s="40"/>
+      <c r="J6" s="40"/>
+      <c r="K6" s="40"/>
+      <c r="L6" s="45"/>
     </row>
     <row r="7" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B7" s="30"/>
@@ -1242,11 +1245,11 @@
       <c r="E8" s="29"/>
       <c r="F8" s="29"/>
       <c r="G8" s="29"/>
-      <c r="H8" s="41" t="s">
+      <c r="H8" s="43" t="s">
         <v>13</v>
       </c>
-      <c r="I8" s="39"/>
-      <c r="J8" s="39"/>
+      <c r="I8" s="40"/>
+      <c r="J8" s="40"/>
       <c r="K8" s="29"/>
     </row>
     <row r="9" spans="2:12" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1539,15 +1542,15 @@
       <c r="H1" s="36"/>
     </row>
     <row r="2" spans="2:8" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="44" t="s">
+      <c r="B2" s="42" t="s">
         <v>34</v>
       </c>
-      <c r="C2" s="39"/>
-      <c r="D2" s="39"/>
-      <c r="E2" s="39"/>
-      <c r="F2" s="39"/>
-      <c r="G2" s="39"/>
-      <c r="H2" s="39"/>
+      <c r="C2" s="40"/>
+      <c r="D2" s="40"/>
+      <c r="E2" s="40"/>
+      <c r="F2" s="40"/>
+      <c r="G2" s="40"/>
+      <c r="H2" s="40"/>
     </row>
     <row r="3" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B3" s="36"/>
@@ -1637,10 +1640,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:BG16"/>
+  <dimension ref="A1:BG18"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="S5" sqref="S5"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Q21" sqref="Q21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1655,7 +1658,8 @@
     <col min="14" max="14" width="8.42578125" customWidth="1"/>
     <col min="15" max="15" width="9.140625" customWidth="1"/>
     <col min="18" max="18" width="9.140625" customWidth="1"/>
-    <col min="20" max="59" width="9.140625" style="1" customWidth="1"/>
+    <col min="20" max="20" width="10.140625" style="48" bestFit="1" customWidth="1"/>
+    <col min="21" max="59" width="9.140625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:22" x14ac:dyDescent="0.25">
@@ -1677,48 +1681,51 @@
       <c r="Q1" s="1"/>
       <c r="R1" s="1"/>
       <c r="S1" s="1"/>
+      <c r="T1" s="1"/>
     </row>
     <row r="2" spans="2:22" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="38" t="s">
+      <c r="B2" s="39" t="s">
         <v>42</v>
       </c>
-      <c r="C2" s="39"/>
-      <c r="D2" s="39"/>
-      <c r="E2" s="39"/>
-      <c r="F2" s="39"/>
-      <c r="G2" s="39"/>
-      <c r="H2" s="39"/>
-      <c r="I2" s="39"/>
-      <c r="J2" s="39"/>
-      <c r="K2" s="39"/>
-      <c r="L2" s="39"/>
-      <c r="M2" s="39"/>
-      <c r="N2" s="39"/>
-      <c r="O2" s="39"/>
-      <c r="P2" s="39"/>
-      <c r="Q2" s="39"/>
-      <c r="R2" s="39"/>
-      <c r="S2" s="39"/>
+      <c r="C2" s="40"/>
+      <c r="D2" s="40"/>
+      <c r="E2" s="40"/>
+      <c r="F2" s="40"/>
+      <c r="G2" s="40"/>
+      <c r="H2" s="40"/>
+      <c r="I2" s="40"/>
+      <c r="J2" s="40"/>
+      <c r="K2" s="40"/>
+      <c r="L2" s="40"/>
+      <c r="M2" s="40"/>
+      <c r="N2" s="40"/>
+      <c r="O2" s="40"/>
+      <c r="P2" s="40"/>
+      <c r="Q2" s="40"/>
+      <c r="R2" s="40"/>
+      <c r="S2" s="40"/>
+      <c r="T2" s="1"/>
     </row>
     <row r="3" spans="2:22" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="39"/>
-      <c r="C3" s="39"/>
-      <c r="D3" s="39"/>
-      <c r="E3" s="39"/>
-      <c r="F3" s="39"/>
-      <c r="G3" s="39"/>
-      <c r="H3" s="39"/>
-      <c r="I3" s="39"/>
-      <c r="J3" s="39"/>
-      <c r="K3" s="39"/>
-      <c r="L3" s="39"/>
-      <c r="M3" s="39"/>
-      <c r="N3" s="39"/>
-      <c r="O3" s="39"/>
-      <c r="P3" s="39"/>
-      <c r="Q3" s="39"/>
-      <c r="R3" s="39"/>
-      <c r="S3" s="39"/>
+      <c r="B3" s="40"/>
+      <c r="C3" s="40"/>
+      <c r="D3" s="40"/>
+      <c r="E3" s="40"/>
+      <c r="F3" s="40"/>
+      <c r="G3" s="40"/>
+      <c r="H3" s="40"/>
+      <c r="I3" s="40"/>
+      <c r="J3" s="40"/>
+      <c r="K3" s="40"/>
+      <c r="L3" s="40"/>
+      <c r="M3" s="40"/>
+      <c r="N3" s="40"/>
+      <c r="O3" s="40"/>
+      <c r="P3" s="40"/>
+      <c r="Q3" s="40"/>
+      <c r="R3" s="40"/>
+      <c r="S3" s="40"/>
+      <c r="T3" s="1"/>
     </row>
     <row r="4" spans="2:22" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="1"/>
@@ -1739,6 +1746,7 @@
       <c r="Q4" s="1"/>
       <c r="R4" s="1"/>
       <c r="S4" s="1"/>
+      <c r="T4" s="1"/>
     </row>
     <row r="5" spans="2:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="10" t="s">
@@ -1795,6 +1803,9 @@
       <c r="S5" s="20" t="s">
         <v>58</v>
       </c>
+      <c r="T5" s="20" t="s">
+        <v>109</v>
+      </c>
     </row>
     <row r="6" spans="2:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
@@ -1852,6 +1863,9 @@
       <c r="S6" s="7">
         <v>0.2</v>
       </c>
+      <c r="T6" s="7">
+        <v>2.5000000000000001E-2</v>
+      </c>
       <c r="V6" s="34" t="s">
         <v>60</v>
       </c>
@@ -1912,6 +1926,9 @@
       <c r="S7" s="7">
         <v>0.2</v>
       </c>
+      <c r="T7" s="7">
+        <v>2.5000000000000001E-2</v>
+      </c>
       <c r="V7" s="34" t="s">
         <v>61</v>
       </c>
@@ -1972,6 +1989,9 @@
       <c r="S8" s="7">
         <v>0.2</v>
       </c>
+      <c r="T8" s="7">
+        <v>2.5000000000000001E-2</v>
+      </c>
       <c r="V8" s="34" t="s">
         <v>62</v>
       </c>
@@ -2032,6 +2052,9 @@
       <c r="S9" s="7">
         <v>0.2</v>
       </c>
+      <c r="T9" s="7">
+        <v>2.5000000000000001E-2</v>
+      </c>
     </row>
     <row r="10" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
@@ -2089,6 +2112,9 @@
       <c r="S10" s="7">
         <v>0.2</v>
       </c>
+      <c r="T10" s="7">
+        <v>2.5000000000000001E-2</v>
+      </c>
     </row>
     <row r="11" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
@@ -2146,6 +2172,9 @@
       <c r="S11" s="7">
         <v>0.2</v>
       </c>
+      <c r="T11" s="7">
+        <v>2.5000000000000001E-2</v>
+      </c>
     </row>
     <row r="12" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
@@ -2206,6 +2235,9 @@
       <c r="S12" s="7">
         <v>0.2</v>
       </c>
+      <c r="T12" s="7">
+        <v>2.5000000000000001E-2</v>
+      </c>
     </row>
     <row r="13" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
@@ -2267,6 +2299,9 @@
       <c r="S13" s="7">
         <v>0.2</v>
       </c>
+      <c r="T13" s="7">
+        <v>2.5000000000000001E-2</v>
+      </c>
     </row>
     <row r="14" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
@@ -2328,6 +2363,9 @@
       <c r="S14" s="7">
         <v>0.2</v>
       </c>
+      <c r="T14" s="7">
+        <v>2.5000000000000001E-2</v>
+      </c>
     </row>
     <row r="15" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
@@ -2389,6 +2427,9 @@
       <c r="S15" s="7">
         <v>0.2</v>
       </c>
+      <c r="T15" s="7">
+        <v>2.5000000000000001E-2</v>
+      </c>
     </row>
     <row r="16" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
@@ -2450,6 +2491,15 @@
       <c r="S16" s="7">
         <v>0.2</v>
       </c>
+      <c r="T16" s="7">
+        <v>2.5000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="20:20" x14ac:dyDescent="0.25">
+      <c r="T17"/>
+    </row>
+    <row r="18" spans="20:20" x14ac:dyDescent="0.25">
+      <c r="T18"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2510,165 +2560,165 @@
       <c r="S1" s="12"/>
     </row>
     <row r="2" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B2" s="46" t="s">
+      <c r="B2" s="47" t="s">
         <v>63</v>
       </c>
-      <c r="C2" s="39"/>
-      <c r="D2" s="39"/>
-      <c r="E2" s="39"/>
-      <c r="F2" s="39"/>
-      <c r="G2" s="39"/>
-      <c r="H2" s="39"/>
-      <c r="I2" s="39"/>
-      <c r="J2" s="39"/>
-      <c r="K2" s="39"/>
-      <c r="L2" s="39"/>
-      <c r="M2" s="39"/>
-      <c r="N2" s="39"/>
-      <c r="O2" s="39"/>
-      <c r="P2" s="39"/>
-      <c r="Q2" s="39"/>
-      <c r="R2" s="39"/>
+      <c r="C2" s="40"/>
+      <c r="D2" s="40"/>
+      <c r="E2" s="40"/>
+      <c r="F2" s="40"/>
+      <c r="G2" s="40"/>
+      <c r="H2" s="40"/>
+      <c r="I2" s="40"/>
+      <c r="J2" s="40"/>
+      <c r="K2" s="40"/>
+      <c r="L2" s="40"/>
+      <c r="M2" s="40"/>
+      <c r="N2" s="40"/>
+      <c r="O2" s="40"/>
+      <c r="P2" s="40"/>
+      <c r="Q2" s="40"/>
+      <c r="R2" s="40"/>
       <c r="S2" s="13"/>
     </row>
     <row r="3" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B3" s="39"/>
-      <c r="C3" s="39"/>
-      <c r="D3" s="39"/>
-      <c r="E3" s="39"/>
-      <c r="F3" s="39"/>
-      <c r="G3" s="39"/>
-      <c r="H3" s="39"/>
-      <c r="I3" s="39"/>
-      <c r="J3" s="39"/>
-      <c r="K3" s="39"/>
-      <c r="L3" s="39"/>
-      <c r="M3" s="39"/>
-      <c r="N3" s="39"/>
-      <c r="O3" s="39"/>
-      <c r="P3" s="39"/>
-      <c r="Q3" s="39"/>
-      <c r="R3" s="39"/>
+      <c r="B3" s="40"/>
+      <c r="C3" s="40"/>
+      <c r="D3" s="40"/>
+      <c r="E3" s="40"/>
+      <c r="F3" s="40"/>
+      <c r="G3" s="40"/>
+      <c r="H3" s="40"/>
+      <c r="I3" s="40"/>
+      <c r="J3" s="40"/>
+      <c r="K3" s="40"/>
+      <c r="L3" s="40"/>
+      <c r="M3" s="40"/>
+      <c r="N3" s="40"/>
+      <c r="O3" s="40"/>
+      <c r="P3" s="40"/>
+      <c r="Q3" s="40"/>
+      <c r="R3" s="40"/>
       <c r="S3" s="13"/>
     </row>
     <row r="4" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B4" s="39"/>
-      <c r="C4" s="39"/>
-      <c r="D4" s="39"/>
-      <c r="E4" s="39"/>
-      <c r="F4" s="39"/>
-      <c r="G4" s="39"/>
-      <c r="H4" s="39"/>
-      <c r="I4" s="39"/>
-      <c r="J4" s="39"/>
-      <c r="K4" s="39"/>
-      <c r="L4" s="39"/>
-      <c r="M4" s="39"/>
-      <c r="N4" s="39"/>
-      <c r="O4" s="39"/>
-      <c r="P4" s="39"/>
-      <c r="Q4" s="39"/>
-      <c r="R4" s="39"/>
+      <c r="B4" s="40"/>
+      <c r="C4" s="40"/>
+      <c r="D4" s="40"/>
+      <c r="E4" s="40"/>
+      <c r="F4" s="40"/>
+      <c r="G4" s="40"/>
+      <c r="H4" s="40"/>
+      <c r="I4" s="40"/>
+      <c r="J4" s="40"/>
+      <c r="K4" s="40"/>
+      <c r="L4" s="40"/>
+      <c r="M4" s="40"/>
+      <c r="N4" s="40"/>
+      <c r="O4" s="40"/>
+      <c r="P4" s="40"/>
+      <c r="Q4" s="40"/>
+      <c r="R4" s="40"/>
       <c r="S4" s="13"/>
     </row>
     <row r="5" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B5" s="39"/>
-      <c r="C5" s="39"/>
-      <c r="D5" s="39"/>
-      <c r="E5" s="39"/>
-      <c r="F5" s="39"/>
-      <c r="G5" s="39"/>
-      <c r="H5" s="39"/>
-      <c r="I5" s="39"/>
-      <c r="J5" s="39"/>
-      <c r="K5" s="39"/>
-      <c r="L5" s="39"/>
-      <c r="M5" s="39"/>
-      <c r="N5" s="39"/>
-      <c r="O5" s="39"/>
-      <c r="P5" s="39"/>
-      <c r="Q5" s="39"/>
-      <c r="R5" s="39"/>
+      <c r="B5" s="40"/>
+      <c r="C5" s="40"/>
+      <c r="D5" s="40"/>
+      <c r="E5" s="40"/>
+      <c r="F5" s="40"/>
+      <c r="G5" s="40"/>
+      <c r="H5" s="40"/>
+      <c r="I5" s="40"/>
+      <c r="J5" s="40"/>
+      <c r="K5" s="40"/>
+      <c r="L5" s="40"/>
+      <c r="M5" s="40"/>
+      <c r="N5" s="40"/>
+      <c r="O5" s="40"/>
+      <c r="P5" s="40"/>
+      <c r="Q5" s="40"/>
+      <c r="R5" s="40"/>
       <c r="S5" s="13"/>
     </row>
     <row r="6" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B6" s="39"/>
-      <c r="C6" s="39"/>
-      <c r="D6" s="39"/>
-      <c r="E6" s="39"/>
-      <c r="F6" s="39"/>
-      <c r="G6" s="39"/>
-      <c r="H6" s="39"/>
-      <c r="I6" s="39"/>
-      <c r="J6" s="39"/>
-      <c r="K6" s="39"/>
-      <c r="L6" s="39"/>
-      <c r="M6" s="39"/>
-      <c r="N6" s="39"/>
-      <c r="O6" s="39"/>
-      <c r="P6" s="39"/>
-      <c r="Q6" s="39"/>
-      <c r="R6" s="39"/>
+      <c r="B6" s="40"/>
+      <c r="C6" s="40"/>
+      <c r="D6" s="40"/>
+      <c r="E6" s="40"/>
+      <c r="F6" s="40"/>
+      <c r="G6" s="40"/>
+      <c r="H6" s="40"/>
+      <c r="I6" s="40"/>
+      <c r="J6" s="40"/>
+      <c r="K6" s="40"/>
+      <c r="L6" s="40"/>
+      <c r="M6" s="40"/>
+      <c r="N6" s="40"/>
+      <c r="O6" s="40"/>
+      <c r="P6" s="40"/>
+      <c r="Q6" s="40"/>
+      <c r="R6" s="40"/>
       <c r="S6" s="13"/>
     </row>
     <row r="7" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B7" s="39"/>
-      <c r="C7" s="39"/>
-      <c r="D7" s="39"/>
-      <c r="E7" s="39"/>
-      <c r="F7" s="39"/>
-      <c r="G7" s="39"/>
-      <c r="H7" s="39"/>
-      <c r="I7" s="39"/>
-      <c r="J7" s="39"/>
-      <c r="K7" s="39"/>
-      <c r="L7" s="39"/>
-      <c r="M7" s="39"/>
-      <c r="N7" s="39"/>
-      <c r="O7" s="39"/>
-      <c r="P7" s="39"/>
-      <c r="Q7" s="39"/>
-      <c r="R7" s="39"/>
+      <c r="B7" s="40"/>
+      <c r="C7" s="40"/>
+      <c r="D7" s="40"/>
+      <c r="E7" s="40"/>
+      <c r="F7" s="40"/>
+      <c r="G7" s="40"/>
+      <c r="H7" s="40"/>
+      <c r="I7" s="40"/>
+      <c r="J7" s="40"/>
+      <c r="K7" s="40"/>
+      <c r="L7" s="40"/>
+      <c r="M7" s="40"/>
+      <c r="N7" s="40"/>
+      <c r="O7" s="40"/>
+      <c r="P7" s="40"/>
+      <c r="Q7" s="40"/>
+      <c r="R7" s="40"/>
       <c r="S7" s="18"/>
     </row>
     <row r="8" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B8" s="39"/>
-      <c r="C8" s="39"/>
-      <c r="D8" s="39"/>
-      <c r="E8" s="39"/>
-      <c r="F8" s="39"/>
-      <c r="G8" s="39"/>
-      <c r="H8" s="39"/>
-      <c r="I8" s="39"/>
-      <c r="J8" s="39"/>
-      <c r="K8" s="39"/>
-      <c r="L8" s="39"/>
-      <c r="M8" s="39"/>
-      <c r="N8" s="39"/>
-      <c r="O8" s="39"/>
-      <c r="P8" s="39"/>
-      <c r="Q8" s="39"/>
-      <c r="R8" s="39"/>
+      <c r="B8" s="40"/>
+      <c r="C8" s="40"/>
+      <c r="D8" s="40"/>
+      <c r="E8" s="40"/>
+      <c r="F8" s="40"/>
+      <c r="G8" s="40"/>
+      <c r="H8" s="40"/>
+      <c r="I8" s="40"/>
+      <c r="J8" s="40"/>
+      <c r="K8" s="40"/>
+      <c r="L8" s="40"/>
+      <c r="M8" s="40"/>
+      <c r="N8" s="40"/>
+      <c r="O8" s="40"/>
+      <c r="P8" s="40"/>
+      <c r="Q8" s="40"/>
+      <c r="R8" s="40"/>
       <c r="S8" s="13"/>
     </row>
     <row r="9" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B9" s="39"/>
-      <c r="C9" s="39"/>
-      <c r="D9" s="39"/>
-      <c r="E9" s="39"/>
-      <c r="F9" s="39"/>
-      <c r="G9" s="39"/>
-      <c r="H9" s="39"/>
-      <c r="I9" s="39"/>
-      <c r="J9" s="39"/>
-      <c r="K9" s="39"/>
-      <c r="L9" s="39"/>
-      <c r="M9" s="39"/>
-      <c r="N9" s="39"/>
-      <c r="O9" s="39"/>
-      <c r="P9" s="39"/>
-      <c r="Q9" s="39"/>
-      <c r="R9" s="39"/>
+      <c r="B9" s="40"/>
+      <c r="C9" s="40"/>
+      <c r="D9" s="40"/>
+      <c r="E9" s="40"/>
+      <c r="F9" s="40"/>
+      <c r="G9" s="40"/>
+      <c r="H9" s="40"/>
+      <c r="I9" s="40"/>
+      <c r="J9" s="40"/>
+      <c r="K9" s="40"/>
+      <c r="L9" s="40"/>
+      <c r="M9" s="40"/>
+      <c r="N9" s="40"/>
+      <c r="O9" s="40"/>
+      <c r="P9" s="40"/>
+      <c r="Q9" s="40"/>
+      <c r="R9" s="40"/>
       <c r="S9" s="13"/>
     </row>
     <row r="10" spans="2:20" x14ac:dyDescent="0.25">
@@ -2701,11 +2751,11 @@
       <c r="E11" s="28" t="s">
         <v>65</v>
       </c>
-      <c r="F11" s="45" t="s">
+      <c r="F11" s="46" t="s">
         <v>66</v>
       </c>
-      <c r="G11" s="39"/>
-      <c r="H11" s="39"/>
+      <c r="G11" s="40"/>
+      <c r="H11" s="40"/>
       <c r="I11" s="28"/>
       <c r="J11" s="28"/>
       <c r="K11" s="28"/>
@@ -2713,11 +2763,11 @@
       <c r="M11" s="11"/>
       <c r="N11" s="11"/>
       <c r="O11" s="11"/>
-      <c r="P11" s="45" t="s">
+      <c r="P11" s="46" t="s">
         <v>67</v>
       </c>
-      <c r="Q11" s="39"/>
-      <c r="R11" s="39"/>
+      <c r="Q11" s="40"/>
+      <c r="R11" s="40"/>
       <c r="S11" s="14"/>
     </row>
     <row r="12" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2861,76 +2911,76 @@
       <c r="I1" s="2"/>
     </row>
     <row r="2" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="38" t="s">
+      <c r="B2" s="39" t="s">
         <v>87</v>
       </c>
-      <c r="C2" s="39"/>
-      <c r="D2" s="39"/>
-      <c r="E2" s="39"/>
-      <c r="F2" s="39"/>
-      <c r="G2" s="39"/>
-      <c r="H2" s="39"/>
-      <c r="I2" s="39"/>
+      <c r="C2" s="40"/>
+      <c r="D2" s="40"/>
+      <c r="E2" s="40"/>
+      <c r="F2" s="40"/>
+      <c r="G2" s="40"/>
+      <c r="H2" s="40"/>
+      <c r="I2" s="40"/>
     </row>
     <row r="3" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B3" s="39"/>
-      <c r="C3" s="39"/>
-      <c r="D3" s="39"/>
-      <c r="E3" s="39"/>
-      <c r="F3" s="39"/>
-      <c r="G3" s="39"/>
-      <c r="H3" s="39"/>
-      <c r="I3" s="39"/>
+      <c r="B3" s="40"/>
+      <c r="C3" s="40"/>
+      <c r="D3" s="40"/>
+      <c r="E3" s="40"/>
+      <c r="F3" s="40"/>
+      <c r="G3" s="40"/>
+      <c r="H3" s="40"/>
+      <c r="I3" s="40"/>
     </row>
     <row r="4" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B4" s="39"/>
-      <c r="C4" s="39"/>
-      <c r="D4" s="39"/>
-      <c r="E4" s="39"/>
-      <c r="F4" s="39"/>
-      <c r="G4" s="39"/>
-      <c r="H4" s="39"/>
-      <c r="I4" s="39"/>
+      <c r="B4" s="40"/>
+      <c r="C4" s="40"/>
+      <c r="D4" s="40"/>
+      <c r="E4" s="40"/>
+      <c r="F4" s="40"/>
+      <c r="G4" s="40"/>
+      <c r="H4" s="40"/>
+      <c r="I4" s="40"/>
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B5" s="39"/>
-      <c r="C5" s="39"/>
-      <c r="D5" s="39"/>
-      <c r="E5" s="39"/>
-      <c r="F5" s="39"/>
-      <c r="G5" s="39"/>
-      <c r="H5" s="39"/>
-      <c r="I5" s="39"/>
+      <c r="B5" s="40"/>
+      <c r="C5" s="40"/>
+      <c r="D5" s="40"/>
+      <c r="E5" s="40"/>
+      <c r="F5" s="40"/>
+      <c r="G5" s="40"/>
+      <c r="H5" s="40"/>
+      <c r="I5" s="40"/>
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B6" s="39"/>
-      <c r="C6" s="39"/>
-      <c r="D6" s="39"/>
-      <c r="E6" s="39"/>
-      <c r="F6" s="39"/>
-      <c r="G6" s="39"/>
-      <c r="H6" s="39"/>
-      <c r="I6" s="39"/>
+      <c r="B6" s="40"/>
+      <c r="C6" s="40"/>
+      <c r="D6" s="40"/>
+      <c r="E6" s="40"/>
+      <c r="F6" s="40"/>
+      <c r="G6" s="40"/>
+      <c r="H6" s="40"/>
+      <c r="I6" s="40"/>
     </row>
     <row r="7" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B7" s="39"/>
-      <c r="C7" s="39"/>
-      <c r="D7" s="39"/>
-      <c r="E7" s="39"/>
-      <c r="F7" s="39"/>
-      <c r="G7" s="39"/>
-      <c r="H7" s="39"/>
-      <c r="I7" s="39"/>
+      <c r="B7" s="40"/>
+      <c r="C7" s="40"/>
+      <c r="D7" s="40"/>
+      <c r="E7" s="40"/>
+      <c r="F7" s="40"/>
+      <c r="G7" s="40"/>
+      <c r="H7" s="40"/>
+      <c r="I7" s="40"/>
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B8" s="39"/>
-      <c r="C8" s="39"/>
-      <c r="D8" s="39"/>
-      <c r="E8" s="39"/>
-      <c r="F8" s="39"/>
-      <c r="G8" s="39"/>
-      <c r="H8" s="39"/>
-      <c r="I8" s="39"/>
+      <c r="B8" s="40"/>
+      <c r="C8" s="40"/>
+      <c r="D8" s="40"/>
+      <c r="E8" s="40"/>
+      <c r="F8" s="40"/>
+      <c r="G8" s="40"/>
+      <c r="H8" s="40"/>
+      <c r="I8" s="40"/>
     </row>
     <row r="9" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B9" s="2"/>
@@ -15332,60 +15382,60 @@
       <c r="H1" s="3"/>
     </row>
     <row r="2" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="38" t="s">
+      <c r="B2" s="39" t="s">
         <v>100</v>
       </c>
-      <c r="C2" s="39"/>
-      <c r="D2" s="39"/>
-      <c r="E2" s="39"/>
-      <c r="F2" s="39"/>
-      <c r="G2" s="39"/>
-      <c r="H2" s="39"/>
+      <c r="C2" s="40"/>
+      <c r="D2" s="40"/>
+      <c r="E2" s="40"/>
+      <c r="F2" s="40"/>
+      <c r="G2" s="40"/>
+      <c r="H2" s="40"/>
     </row>
     <row r="3" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B3" s="39"/>
-      <c r="C3" s="39"/>
-      <c r="D3" s="39"/>
-      <c r="E3" s="39"/>
-      <c r="F3" s="39"/>
-      <c r="G3" s="39"/>
-      <c r="H3" s="39"/>
+      <c r="B3" s="40"/>
+      <c r="C3" s="40"/>
+      <c r="D3" s="40"/>
+      <c r="E3" s="40"/>
+      <c r="F3" s="40"/>
+      <c r="G3" s="40"/>
+      <c r="H3" s="40"/>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B4" s="39"/>
-      <c r="C4" s="39"/>
-      <c r="D4" s="39"/>
-      <c r="E4" s="39"/>
-      <c r="F4" s="39"/>
-      <c r="G4" s="39"/>
-      <c r="H4" s="39"/>
+      <c r="B4" s="40"/>
+      <c r="C4" s="40"/>
+      <c r="D4" s="40"/>
+      <c r="E4" s="40"/>
+      <c r="F4" s="40"/>
+      <c r="G4" s="40"/>
+      <c r="H4" s="40"/>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B5" s="39"/>
-      <c r="C5" s="39"/>
-      <c r="D5" s="39"/>
-      <c r="E5" s="39"/>
-      <c r="F5" s="39"/>
-      <c r="G5" s="39"/>
-      <c r="H5" s="39"/>
+      <c r="B5" s="40"/>
+      <c r="C5" s="40"/>
+      <c r="D5" s="40"/>
+      <c r="E5" s="40"/>
+      <c r="F5" s="40"/>
+      <c r="G5" s="40"/>
+      <c r="H5" s="40"/>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B6" s="39"/>
-      <c r="C6" s="39"/>
-      <c r="D6" s="39"/>
-      <c r="E6" s="39"/>
-      <c r="F6" s="39"/>
-      <c r="G6" s="39"/>
-      <c r="H6" s="39"/>
+      <c r="B6" s="40"/>
+      <c r="C6" s="40"/>
+      <c r="D6" s="40"/>
+      <c r="E6" s="40"/>
+      <c r="F6" s="40"/>
+      <c r="G6" s="40"/>
+      <c r="H6" s="40"/>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B7" s="39"/>
-      <c r="C7" s="39"/>
-      <c r="D7" s="39"/>
-      <c r="E7" s="39"/>
-      <c r="F7" s="39"/>
-      <c r="G7" s="39"/>
-      <c r="H7" s="39"/>
+      <c r="B7" s="40"/>
+      <c r="C7" s="40"/>
+      <c r="D7" s="40"/>
+      <c r="E7" s="40"/>
+      <c r="F7" s="40"/>
+      <c r="G7" s="40"/>
+      <c r="H7" s="40"/>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B8" s="3"/>

</xml_diff>

<commit_message>
cleaning up code new spreadsheet
</commit_message>
<xml_diff>
--- a/Spreadsheet Interface/Input_Spreadsheet_v250123.xlsx
+++ b/Spreadsheet Interface/Input_Spreadsheet_v250123.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://kleinschmidtgroup-my.sharepoint.com/personal/kevin_nebiolo_kleinschmidtgroup_com/Documents/Software/stryke/Spreadsheet Interface/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A6B91651-D364-4E5F-AC61-FFEA3897CD02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="8_{A6B91651-D364-4E5F-AC61-FFEA3897CD02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{610A50B9-E3B1-4EF1-800C-67F5F0AAB5BC}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19200" yWindow="0" windowWidth="19200" windowHeight="21000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Flow Scenarios" sheetId="1" r:id="rId1"/>
     <sheet name="Hydrology" sheetId="8" r:id="rId2"/>
-    <sheet name="Operating Scenarios" sheetId="2" r:id="rId3"/>
-    <sheet name="Facilities" sheetId="3" r:id="rId4"/>
+    <sheet name="Facilities" sheetId="3" r:id="rId3"/>
+    <sheet name="Operating Scenarios" sheetId="2" r:id="rId4"/>
     <sheet name="Unit Params" sheetId="4" r:id="rId5"/>
     <sheet name="Population" sheetId="5" r:id="rId6"/>
     <sheet name="Nodes" sheetId="6" r:id="rId7"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="110">
   <si>
     <t>Scenario Number</t>
   </si>
@@ -368,6 +368,9 @@
   <si>
     <t xml:space="preserve">This sheet contains information that describe facility discharge.  The end user can either pass a stable discharge into the flow column, or type 'hydrograph'.  If the End User is in the United States and would like to fetch data from a particular USGS Gage and discharge year, enter the gage ID into the Gage column.  If the end user is in Canada, or there is no Gage ID, they will leave the Gage column blank and either use a hard coded stable discharge, or import their own gage data into the Hydrology tab.  The prorate column increases or decreases discharge based on difference in watersheds.  </t>
   </si>
+  <si>
+    <t>cms</t>
+  </si>
 </sst>
 </file>
 
@@ -526,7 +529,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -599,11 +602,15 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -611,17 +618,12 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -938,8 +940,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AZ7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K22" sqref="K22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -966,36 +968,36 @@
       <c r="I1" s="4"/>
     </row>
     <row r="2" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="38" t="s">
+      <c r="B2" s="39" t="s">
         <v>108</v>
       </c>
-      <c r="C2" s="39"/>
-      <c r="D2" s="39"/>
-      <c r="E2" s="40"/>
-      <c r="F2" s="39"/>
-      <c r="G2" s="39"/>
-      <c r="H2" s="39"/>
-      <c r="I2" s="39"/>
+      <c r="C2" s="40"/>
+      <c r="D2" s="40"/>
+      <c r="E2" s="41"/>
+      <c r="F2" s="40"/>
+      <c r="G2" s="40"/>
+      <c r="H2" s="40"/>
+      <c r="I2" s="40"/>
     </row>
     <row r="3" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B3" s="39"/>
-      <c r="C3" s="39"/>
-      <c r="D3" s="39"/>
-      <c r="E3" s="40"/>
-      <c r="F3" s="39"/>
-      <c r="G3" s="39"/>
-      <c r="H3" s="39"/>
-      <c r="I3" s="39"/>
+      <c r="B3" s="40"/>
+      <c r="C3" s="40"/>
+      <c r="D3" s="40"/>
+      <c r="E3" s="41"/>
+      <c r="F3" s="40"/>
+      <c r="G3" s="40"/>
+      <c r="H3" s="40"/>
+      <c r="I3" s="40"/>
     </row>
     <row r="4" spans="2:9" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="39"/>
-      <c r="C4" s="39"/>
-      <c r="D4" s="39"/>
-      <c r="E4" s="40"/>
-      <c r="F4" s="39"/>
-      <c r="G4" s="39"/>
-      <c r="H4" s="39"/>
-      <c r="I4" s="39"/>
+      <c r="B4" s="40"/>
+      <c r="C4" s="40"/>
+      <c r="D4" s="40"/>
+      <c r="E4" s="41"/>
+      <c r="F4" s="40"/>
+      <c r="G4" s="40"/>
+      <c r="H4" s="40"/>
+      <c r="I4" s="40"/>
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B5" s="5"/>
@@ -1072,37 +1074,37 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E087547D-FA44-4C88-A5AA-84196B3A184F}">
   <dimension ref="A1:AK4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="47"/>
+    <col min="1" max="1" width="9.140625" style="38"/>
     <col min="3" max="3" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="37" width="9.140625" style="47"/>
+    <col min="4" max="37" width="9.140625" style="38"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B1" s="47"/>
-      <c r="C1" s="47"/>
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
     </row>
     <row r="2" spans="2:10" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="44" t="s">
+      <c r="B2" s="42" t="s">
         <v>107</v>
       </c>
-      <c r="C2" s="44"/>
-      <c r="D2" s="44"/>
-      <c r="E2" s="44"/>
-      <c r="F2" s="44"/>
-      <c r="G2" s="44"/>
-      <c r="H2" s="44"/>
-      <c r="I2" s="44"/>
-      <c r="J2" s="44"/>
+      <c r="C2" s="42"/>
+      <c r="D2" s="42"/>
+      <c r="E2" s="42"/>
+      <c r="F2" s="42"/>
+      <c r="G2" s="42"/>
+      <c r="H2" s="42"/>
+      <c r="I2" s="42"/>
+      <c r="J2" s="42"/>
     </row>
     <row r="3" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B3" s="47"/>
-      <c r="C3" s="47"/>
+      <c r="B3" s="38"/>
+      <c r="C3" s="38"/>
     </row>
     <row r="4" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B4" s="37" t="s">
@@ -1111,10 +1113,12 @@
       <c r="C4" s="37" t="s">
         <v>105</v>
       </c>
-      <c r="E4" s="48" t="s">
+      <c r="E4" t="s">
         <v>106</v>
       </c>
-      <c r="F4" s="48"/>
+      <c r="F4" t="s">
+        <v>109</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1125,6 +1129,131 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:BI6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="36" customWidth="1"/>
+    <col min="2" max="3" width="12.7109375" customWidth="1"/>
+    <col min="4" max="4" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="61" width="9.140625" style="36" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="36"/>
+      <c r="H1" s="36"/>
+    </row>
+    <row r="2" spans="2:8" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="42" t="s">
+        <v>34</v>
+      </c>
+      <c r="C2" s="40"/>
+      <c r="D2" s="40"/>
+      <c r="E2" s="40"/>
+      <c r="F2" s="40"/>
+      <c r="G2" s="40"/>
+      <c r="H2" s="40"/>
+    </row>
+    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B3" s="36"/>
+      <c r="C3" s="36"/>
+      <c r="D3" s="36"/>
+      <c r="E3" s="36"/>
+      <c r="F3" s="36"/>
+      <c r="G3" s="36"/>
+      <c r="H3" s="36"/>
+    </row>
+    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B4" s="37" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="37" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="37" t="s">
+        <v>35</v>
+      </c>
+      <c r="E4" s="37" t="s">
+        <v>36</v>
+      </c>
+      <c r="F4" s="37" t="s">
+        <v>37</v>
+      </c>
+      <c r="G4" s="37" t="s">
+        <v>38</v>
+      </c>
+      <c r="H4" s="37" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" t="s">
+        <v>40</v>
+      </c>
+      <c r="E5">
+        <v>1200</v>
+      </c>
+      <c r="F5">
+        <v>400</v>
+      </c>
+      <c r="G5">
+        <v>100</v>
+      </c>
+      <c r="H5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" t="s">
+        <v>40</v>
+      </c>
+      <c r="E6">
+        <v>250</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6" t="s">
+        <v>41</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B2:H2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:BC20"/>
   <sheetViews>
@@ -1156,71 +1285,71 @@
       <c r="K1" s="29"/>
     </row>
     <row r="2" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B2" s="42" t="s">
+      <c r="B2" s="44" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="39"/>
-      <c r="D2" s="39"/>
-      <c r="E2" s="39"/>
-      <c r="F2" s="39"/>
-      <c r="G2" s="39"/>
-      <c r="H2" s="39"/>
-      <c r="I2" s="39"/>
-      <c r="J2" s="39"/>
-      <c r="K2" s="39"/>
-      <c r="L2" s="43"/>
+      <c r="C2" s="40"/>
+      <c r="D2" s="40"/>
+      <c r="E2" s="40"/>
+      <c r="F2" s="40"/>
+      <c r="G2" s="40"/>
+      <c r="H2" s="40"/>
+      <c r="I2" s="40"/>
+      <c r="J2" s="40"/>
+      <c r="K2" s="40"/>
+      <c r="L2" s="45"/>
     </row>
     <row r="3" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B3" s="39"/>
-      <c r="C3" s="39"/>
-      <c r="D3" s="39"/>
-      <c r="E3" s="39"/>
-      <c r="F3" s="39"/>
-      <c r="G3" s="39"/>
-      <c r="H3" s="39"/>
-      <c r="I3" s="39"/>
-      <c r="J3" s="39"/>
-      <c r="K3" s="39"/>
-      <c r="L3" s="43"/>
+      <c r="B3" s="40"/>
+      <c r="C3" s="40"/>
+      <c r="D3" s="40"/>
+      <c r="E3" s="40"/>
+      <c r="F3" s="40"/>
+      <c r="G3" s="40"/>
+      <c r="H3" s="40"/>
+      <c r="I3" s="40"/>
+      <c r="J3" s="40"/>
+      <c r="K3" s="40"/>
+      <c r="L3" s="45"/>
     </row>
     <row r="4" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B4" s="39"/>
-      <c r="C4" s="39"/>
-      <c r="D4" s="39"/>
-      <c r="E4" s="39"/>
-      <c r="F4" s="39"/>
-      <c r="G4" s="39"/>
-      <c r="H4" s="39"/>
-      <c r="I4" s="39"/>
-      <c r="J4" s="39"/>
-      <c r="K4" s="39"/>
-      <c r="L4" s="43"/>
+      <c r="B4" s="40"/>
+      <c r="C4" s="40"/>
+      <c r="D4" s="40"/>
+      <c r="E4" s="40"/>
+      <c r="F4" s="40"/>
+      <c r="G4" s="40"/>
+      <c r="H4" s="40"/>
+      <c r="I4" s="40"/>
+      <c r="J4" s="40"/>
+      <c r="K4" s="40"/>
+      <c r="L4" s="45"/>
     </row>
     <row r="5" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B5" s="39"/>
-      <c r="C5" s="39"/>
-      <c r="D5" s="39"/>
-      <c r="E5" s="39"/>
-      <c r="F5" s="39"/>
-      <c r="G5" s="39"/>
-      <c r="H5" s="39"/>
-      <c r="I5" s="39"/>
-      <c r="J5" s="39"/>
-      <c r="K5" s="39"/>
-      <c r="L5" s="43"/>
+      <c r="B5" s="40"/>
+      <c r="C5" s="40"/>
+      <c r="D5" s="40"/>
+      <c r="E5" s="40"/>
+      <c r="F5" s="40"/>
+      <c r="G5" s="40"/>
+      <c r="H5" s="40"/>
+      <c r="I5" s="40"/>
+      <c r="J5" s="40"/>
+      <c r="K5" s="40"/>
+      <c r="L5" s="45"/>
     </row>
     <row r="6" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B6" s="39"/>
-      <c r="C6" s="39"/>
-      <c r="D6" s="39"/>
-      <c r="E6" s="39"/>
-      <c r="F6" s="39"/>
-      <c r="G6" s="39"/>
-      <c r="H6" s="39"/>
-      <c r="I6" s="39"/>
-      <c r="J6" s="39"/>
-      <c r="K6" s="39"/>
-      <c r="L6" s="43"/>
+      <c r="B6" s="40"/>
+      <c r="C6" s="40"/>
+      <c r="D6" s="40"/>
+      <c r="E6" s="40"/>
+      <c r="F6" s="40"/>
+      <c r="G6" s="40"/>
+      <c r="H6" s="40"/>
+      <c r="I6" s="40"/>
+      <c r="J6" s="40"/>
+      <c r="K6" s="40"/>
+      <c r="L6" s="45"/>
     </row>
     <row r="7" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B7" s="30"/>
@@ -1242,11 +1371,11 @@
       <c r="E8" s="29"/>
       <c r="F8" s="29"/>
       <c r="G8" s="29"/>
-      <c r="H8" s="41" t="s">
+      <c r="H8" s="43" t="s">
         <v>13</v>
       </c>
-      <c r="I8" s="39"/>
-      <c r="J8" s="39"/>
+      <c r="I8" s="40"/>
+      <c r="J8" s="40"/>
       <c r="K8" s="29"/>
     </row>
     <row r="9" spans="2:12" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1505,131 +1634,6 @@
   <mergeCells count="2">
     <mergeCell ref="H8:J8"/>
     <mergeCell ref="B2:L6"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:BI6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="9.140625" style="36" customWidth="1"/>
-    <col min="2" max="3" width="12.7109375" customWidth="1"/>
-    <col min="4" max="4" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="61" width="9.140625" style="36" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B1" s="36"/>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36"/>
-      <c r="E1" s="36"/>
-      <c r="F1" s="36"/>
-      <c r="G1" s="36"/>
-      <c r="H1" s="36"/>
-    </row>
-    <row r="2" spans="2:8" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="44" t="s">
-        <v>34</v>
-      </c>
-      <c r="C2" s="39"/>
-      <c r="D2" s="39"/>
-      <c r="E2" s="39"/>
-      <c r="F2" s="39"/>
-      <c r="G2" s="39"/>
-      <c r="H2" s="39"/>
-    </row>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B3" s="36"/>
-      <c r="C3" s="36"/>
-      <c r="D3" s="36"/>
-      <c r="E3" s="36"/>
-      <c r="F3" s="36"/>
-      <c r="G3" s="36"/>
-      <c r="H3" s="36"/>
-    </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B4" s="37" t="s">
-        <v>14</v>
-      </c>
-      <c r="C4" s="37" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" s="37" t="s">
-        <v>35</v>
-      </c>
-      <c r="E4" s="37" t="s">
-        <v>36</v>
-      </c>
-      <c r="F4" s="37" t="s">
-        <v>37</v>
-      </c>
-      <c r="G4" s="37" t="s">
-        <v>38</v>
-      </c>
-      <c r="H4" s="37" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D5" t="s">
-        <v>40</v>
-      </c>
-      <c r="E5">
-        <v>1200</v>
-      </c>
-      <c r="F5">
-        <v>400</v>
-      </c>
-      <c r="G5">
-        <v>100</v>
-      </c>
-      <c r="H5" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
-        <v>28</v>
-      </c>
-      <c r="C6" t="s">
-        <v>8</v>
-      </c>
-      <c r="D6" t="s">
-        <v>40</v>
-      </c>
-      <c r="E6">
-        <v>250</v>
-      </c>
-      <c r="F6">
-        <v>0</v>
-      </c>
-      <c r="G6">
-        <v>0</v>
-      </c>
-      <c r="H6" t="s">
-        <v>41</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="B2:H2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1679,46 +1683,46 @@
       <c r="S1" s="1"/>
     </row>
     <row r="2" spans="2:22" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="38" t="s">
+      <c r="B2" s="39" t="s">
         <v>42</v>
       </c>
-      <c r="C2" s="39"/>
-      <c r="D2" s="39"/>
-      <c r="E2" s="39"/>
-      <c r="F2" s="39"/>
-      <c r="G2" s="39"/>
-      <c r="H2" s="39"/>
-      <c r="I2" s="39"/>
-      <c r="J2" s="39"/>
-      <c r="K2" s="39"/>
-      <c r="L2" s="39"/>
-      <c r="M2" s="39"/>
-      <c r="N2" s="39"/>
-      <c r="O2" s="39"/>
-      <c r="P2" s="39"/>
-      <c r="Q2" s="39"/>
-      <c r="R2" s="39"/>
-      <c r="S2" s="39"/>
+      <c r="C2" s="40"/>
+      <c r="D2" s="40"/>
+      <c r="E2" s="40"/>
+      <c r="F2" s="40"/>
+      <c r="G2" s="40"/>
+      <c r="H2" s="40"/>
+      <c r="I2" s="40"/>
+      <c r="J2" s="40"/>
+      <c r="K2" s="40"/>
+      <c r="L2" s="40"/>
+      <c r="M2" s="40"/>
+      <c r="N2" s="40"/>
+      <c r="O2" s="40"/>
+      <c r="P2" s="40"/>
+      <c r="Q2" s="40"/>
+      <c r="R2" s="40"/>
+      <c r="S2" s="40"/>
     </row>
     <row r="3" spans="2:22" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="39"/>
-      <c r="C3" s="39"/>
-      <c r="D3" s="39"/>
-      <c r="E3" s="39"/>
-      <c r="F3" s="39"/>
-      <c r="G3" s="39"/>
-      <c r="H3" s="39"/>
-      <c r="I3" s="39"/>
-      <c r="J3" s="39"/>
-      <c r="K3" s="39"/>
-      <c r="L3" s="39"/>
-      <c r="M3" s="39"/>
-      <c r="N3" s="39"/>
-      <c r="O3" s="39"/>
-      <c r="P3" s="39"/>
-      <c r="Q3" s="39"/>
-      <c r="R3" s="39"/>
-      <c r="S3" s="39"/>
+      <c r="B3" s="40"/>
+      <c r="C3" s="40"/>
+      <c r="D3" s="40"/>
+      <c r="E3" s="40"/>
+      <c r="F3" s="40"/>
+      <c r="G3" s="40"/>
+      <c r="H3" s="40"/>
+      <c r="I3" s="40"/>
+      <c r="J3" s="40"/>
+      <c r="K3" s="40"/>
+      <c r="L3" s="40"/>
+      <c r="M3" s="40"/>
+      <c r="N3" s="40"/>
+      <c r="O3" s="40"/>
+      <c r="P3" s="40"/>
+      <c r="Q3" s="40"/>
+      <c r="R3" s="40"/>
+      <c r="S3" s="40"/>
     </row>
     <row r="4" spans="2:22" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="1"/>
@@ -2510,165 +2514,165 @@
       <c r="S1" s="12"/>
     </row>
     <row r="2" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B2" s="46" t="s">
+      <c r="B2" s="47" t="s">
         <v>63</v>
       </c>
-      <c r="C2" s="39"/>
-      <c r="D2" s="39"/>
-      <c r="E2" s="39"/>
-      <c r="F2" s="39"/>
-      <c r="G2" s="39"/>
-      <c r="H2" s="39"/>
-      <c r="I2" s="39"/>
-      <c r="J2" s="39"/>
-      <c r="K2" s="39"/>
-      <c r="L2" s="39"/>
-      <c r="M2" s="39"/>
-      <c r="N2" s="39"/>
-      <c r="O2" s="39"/>
-      <c r="P2" s="39"/>
-      <c r="Q2" s="39"/>
-      <c r="R2" s="39"/>
+      <c r="C2" s="40"/>
+      <c r="D2" s="40"/>
+      <c r="E2" s="40"/>
+      <c r="F2" s="40"/>
+      <c r="G2" s="40"/>
+      <c r="H2" s="40"/>
+      <c r="I2" s="40"/>
+      <c r="J2" s="40"/>
+      <c r="K2" s="40"/>
+      <c r="L2" s="40"/>
+      <c r="M2" s="40"/>
+      <c r="N2" s="40"/>
+      <c r="O2" s="40"/>
+      <c r="P2" s="40"/>
+      <c r="Q2" s="40"/>
+      <c r="R2" s="40"/>
       <c r="S2" s="13"/>
     </row>
     <row r="3" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B3" s="39"/>
-      <c r="C3" s="39"/>
-      <c r="D3" s="39"/>
-      <c r="E3" s="39"/>
-      <c r="F3" s="39"/>
-      <c r="G3" s="39"/>
-      <c r="H3" s="39"/>
-      <c r="I3" s="39"/>
-      <c r="J3" s="39"/>
-      <c r="K3" s="39"/>
-      <c r="L3" s="39"/>
-      <c r="M3" s="39"/>
-      <c r="N3" s="39"/>
-      <c r="O3" s="39"/>
-      <c r="P3" s="39"/>
-      <c r="Q3" s="39"/>
-      <c r="R3" s="39"/>
+      <c r="B3" s="40"/>
+      <c r="C3" s="40"/>
+      <c r="D3" s="40"/>
+      <c r="E3" s="40"/>
+      <c r="F3" s="40"/>
+      <c r="G3" s="40"/>
+      <c r="H3" s="40"/>
+      <c r="I3" s="40"/>
+      <c r="J3" s="40"/>
+      <c r="K3" s="40"/>
+      <c r="L3" s="40"/>
+      <c r="M3" s="40"/>
+      <c r="N3" s="40"/>
+      <c r="O3" s="40"/>
+      <c r="P3" s="40"/>
+      <c r="Q3" s="40"/>
+      <c r="R3" s="40"/>
       <c r="S3" s="13"/>
     </row>
     <row r="4" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B4" s="39"/>
-      <c r="C4" s="39"/>
-      <c r="D4" s="39"/>
-      <c r="E4" s="39"/>
-      <c r="F4" s="39"/>
-      <c r="G4" s="39"/>
-      <c r="H4" s="39"/>
-      <c r="I4" s="39"/>
-      <c r="J4" s="39"/>
-      <c r="K4" s="39"/>
-      <c r="L4" s="39"/>
-      <c r="M4" s="39"/>
-      <c r="N4" s="39"/>
-      <c r="O4" s="39"/>
-      <c r="P4" s="39"/>
-      <c r="Q4" s="39"/>
-      <c r="R4" s="39"/>
+      <c r="B4" s="40"/>
+      <c r="C4" s="40"/>
+      <c r="D4" s="40"/>
+      <c r="E4" s="40"/>
+      <c r="F4" s="40"/>
+      <c r="G4" s="40"/>
+      <c r="H4" s="40"/>
+      <c r="I4" s="40"/>
+      <c r="J4" s="40"/>
+      <c r="K4" s="40"/>
+      <c r="L4" s="40"/>
+      <c r="M4" s="40"/>
+      <c r="N4" s="40"/>
+      <c r="O4" s="40"/>
+      <c r="P4" s="40"/>
+      <c r="Q4" s="40"/>
+      <c r="R4" s="40"/>
       <c r="S4" s="13"/>
     </row>
     <row r="5" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B5" s="39"/>
-      <c r="C5" s="39"/>
-      <c r="D5" s="39"/>
-      <c r="E5" s="39"/>
-      <c r="F5" s="39"/>
-      <c r="G5" s="39"/>
-      <c r="H5" s="39"/>
-      <c r="I5" s="39"/>
-      <c r="J5" s="39"/>
-      <c r="K5" s="39"/>
-      <c r="L5" s="39"/>
-      <c r="M5" s="39"/>
-      <c r="N5" s="39"/>
-      <c r="O5" s="39"/>
-      <c r="P5" s="39"/>
-      <c r="Q5" s="39"/>
-      <c r="R5" s="39"/>
+      <c r="B5" s="40"/>
+      <c r="C5" s="40"/>
+      <c r="D5" s="40"/>
+      <c r="E5" s="40"/>
+      <c r="F5" s="40"/>
+      <c r="G5" s="40"/>
+      <c r="H5" s="40"/>
+      <c r="I5" s="40"/>
+      <c r="J5" s="40"/>
+      <c r="K5" s="40"/>
+      <c r="L5" s="40"/>
+      <c r="M5" s="40"/>
+      <c r="N5" s="40"/>
+      <c r="O5" s="40"/>
+      <c r="P5" s="40"/>
+      <c r="Q5" s="40"/>
+      <c r="R5" s="40"/>
       <c r="S5" s="13"/>
     </row>
     <row r="6" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B6" s="39"/>
-      <c r="C6" s="39"/>
-      <c r="D6" s="39"/>
-      <c r="E6" s="39"/>
-      <c r="F6" s="39"/>
-      <c r="G6" s="39"/>
-      <c r="H6" s="39"/>
-      <c r="I6" s="39"/>
-      <c r="J6" s="39"/>
-      <c r="K6" s="39"/>
-      <c r="L6" s="39"/>
-      <c r="M6" s="39"/>
-      <c r="N6" s="39"/>
-      <c r="O6" s="39"/>
-      <c r="P6" s="39"/>
-      <c r="Q6" s="39"/>
-      <c r="R6" s="39"/>
+      <c r="B6" s="40"/>
+      <c r="C6" s="40"/>
+      <c r="D6" s="40"/>
+      <c r="E6" s="40"/>
+      <c r="F6" s="40"/>
+      <c r="G6" s="40"/>
+      <c r="H6" s="40"/>
+      <c r="I6" s="40"/>
+      <c r="J6" s="40"/>
+      <c r="K6" s="40"/>
+      <c r="L6" s="40"/>
+      <c r="M6" s="40"/>
+      <c r="N6" s="40"/>
+      <c r="O6" s="40"/>
+      <c r="P6" s="40"/>
+      <c r="Q6" s="40"/>
+      <c r="R6" s="40"/>
       <c r="S6" s="13"/>
     </row>
     <row r="7" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B7" s="39"/>
-      <c r="C7" s="39"/>
-      <c r="D7" s="39"/>
-      <c r="E7" s="39"/>
-      <c r="F7" s="39"/>
-      <c r="G7" s="39"/>
-      <c r="H7" s="39"/>
-      <c r="I7" s="39"/>
-      <c r="J7" s="39"/>
-      <c r="K7" s="39"/>
-      <c r="L7" s="39"/>
-      <c r="M7" s="39"/>
-      <c r="N7" s="39"/>
-      <c r="O7" s="39"/>
-      <c r="P7" s="39"/>
-      <c r="Q7" s="39"/>
-      <c r="R7" s="39"/>
+      <c r="B7" s="40"/>
+      <c r="C7" s="40"/>
+      <c r="D7" s="40"/>
+      <c r="E7" s="40"/>
+      <c r="F7" s="40"/>
+      <c r="G7" s="40"/>
+      <c r="H7" s="40"/>
+      <c r="I7" s="40"/>
+      <c r="J7" s="40"/>
+      <c r="K7" s="40"/>
+      <c r="L7" s="40"/>
+      <c r="M7" s="40"/>
+      <c r="N7" s="40"/>
+      <c r="O7" s="40"/>
+      <c r="P7" s="40"/>
+      <c r="Q7" s="40"/>
+      <c r="R7" s="40"/>
       <c r="S7" s="18"/>
     </row>
     <row r="8" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B8" s="39"/>
-      <c r="C8" s="39"/>
-      <c r="D8" s="39"/>
-      <c r="E8" s="39"/>
-      <c r="F8" s="39"/>
-      <c r="G8" s="39"/>
-      <c r="H8" s="39"/>
-      <c r="I8" s="39"/>
-      <c r="J8" s="39"/>
-      <c r="K8" s="39"/>
-      <c r="L8" s="39"/>
-      <c r="M8" s="39"/>
-      <c r="N8" s="39"/>
-      <c r="O8" s="39"/>
-      <c r="P8" s="39"/>
-      <c r="Q8" s="39"/>
-      <c r="R8" s="39"/>
+      <c r="B8" s="40"/>
+      <c r="C8" s="40"/>
+      <c r="D8" s="40"/>
+      <c r="E8" s="40"/>
+      <c r="F8" s="40"/>
+      <c r="G8" s="40"/>
+      <c r="H8" s="40"/>
+      <c r="I8" s="40"/>
+      <c r="J8" s="40"/>
+      <c r="K8" s="40"/>
+      <c r="L8" s="40"/>
+      <c r="M8" s="40"/>
+      <c r="N8" s="40"/>
+      <c r="O8" s="40"/>
+      <c r="P8" s="40"/>
+      <c r="Q8" s="40"/>
+      <c r="R8" s="40"/>
       <c r="S8" s="13"/>
     </row>
     <row r="9" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B9" s="39"/>
-      <c r="C9" s="39"/>
-      <c r="D9" s="39"/>
-      <c r="E9" s="39"/>
-      <c r="F9" s="39"/>
-      <c r="G9" s="39"/>
-      <c r="H9" s="39"/>
-      <c r="I9" s="39"/>
-      <c r="J9" s="39"/>
-      <c r="K9" s="39"/>
-      <c r="L9" s="39"/>
-      <c r="M9" s="39"/>
-      <c r="N9" s="39"/>
-      <c r="O9" s="39"/>
-      <c r="P9" s="39"/>
-      <c r="Q9" s="39"/>
-      <c r="R9" s="39"/>
+      <c r="B9" s="40"/>
+      <c r="C9" s="40"/>
+      <c r="D9" s="40"/>
+      <c r="E9" s="40"/>
+      <c r="F9" s="40"/>
+      <c r="G9" s="40"/>
+      <c r="H9" s="40"/>
+      <c r="I9" s="40"/>
+      <c r="J9" s="40"/>
+      <c r="K9" s="40"/>
+      <c r="L9" s="40"/>
+      <c r="M9" s="40"/>
+      <c r="N9" s="40"/>
+      <c r="O9" s="40"/>
+      <c r="P9" s="40"/>
+      <c r="Q9" s="40"/>
+      <c r="R9" s="40"/>
       <c r="S9" s="13"/>
     </row>
     <row r="10" spans="2:20" x14ac:dyDescent="0.25">
@@ -2701,11 +2705,11 @@
       <c r="E11" s="28" t="s">
         <v>65</v>
       </c>
-      <c r="F11" s="45" t="s">
+      <c r="F11" s="46" t="s">
         <v>66</v>
       </c>
-      <c r="G11" s="39"/>
-      <c r="H11" s="39"/>
+      <c r="G11" s="40"/>
+      <c r="H11" s="40"/>
       <c r="I11" s="28"/>
       <c r="J11" s="28"/>
       <c r="K11" s="28"/>
@@ -2713,11 +2717,11 @@
       <c r="M11" s="11"/>
       <c r="N11" s="11"/>
       <c r="O11" s="11"/>
-      <c r="P11" s="45" t="s">
+      <c r="P11" s="46" t="s">
         <v>67</v>
       </c>
-      <c r="Q11" s="39"/>
-      <c r="R11" s="39"/>
+      <c r="Q11" s="40"/>
+      <c r="R11" s="40"/>
       <c r="S11" s="14"/>
     </row>
     <row r="12" spans="2:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2861,76 +2865,76 @@
       <c r="I1" s="2"/>
     </row>
     <row r="2" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="38" t="s">
+      <c r="B2" s="39" t="s">
         <v>87</v>
       </c>
-      <c r="C2" s="39"/>
-      <c r="D2" s="39"/>
-      <c r="E2" s="39"/>
-      <c r="F2" s="39"/>
-      <c r="G2" s="39"/>
-      <c r="H2" s="39"/>
-      <c r="I2" s="39"/>
+      <c r="C2" s="40"/>
+      <c r="D2" s="40"/>
+      <c r="E2" s="40"/>
+      <c r="F2" s="40"/>
+      <c r="G2" s="40"/>
+      <c r="H2" s="40"/>
+      <c r="I2" s="40"/>
     </row>
     <row r="3" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B3" s="39"/>
-      <c r="C3" s="39"/>
-      <c r="D3" s="39"/>
-      <c r="E3" s="39"/>
-      <c r="F3" s="39"/>
-      <c r="G3" s="39"/>
-      <c r="H3" s="39"/>
-      <c r="I3" s="39"/>
+      <c r="B3" s="40"/>
+      <c r="C3" s="40"/>
+      <c r="D3" s="40"/>
+      <c r="E3" s="40"/>
+      <c r="F3" s="40"/>
+      <c r="G3" s="40"/>
+      <c r="H3" s="40"/>
+      <c r="I3" s="40"/>
     </row>
     <row r="4" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B4" s="39"/>
-      <c r="C4" s="39"/>
-      <c r="D4" s="39"/>
-      <c r="E4" s="39"/>
-      <c r="F4" s="39"/>
-      <c r="G4" s="39"/>
-      <c r="H4" s="39"/>
-      <c r="I4" s="39"/>
+      <c r="B4" s="40"/>
+      <c r="C4" s="40"/>
+      <c r="D4" s="40"/>
+      <c r="E4" s="40"/>
+      <c r="F4" s="40"/>
+      <c r="G4" s="40"/>
+      <c r="H4" s="40"/>
+      <c r="I4" s="40"/>
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B5" s="39"/>
-      <c r="C5" s="39"/>
-      <c r="D5" s="39"/>
-      <c r="E5" s="39"/>
-      <c r="F5" s="39"/>
-      <c r="G5" s="39"/>
-      <c r="H5" s="39"/>
-      <c r="I5" s="39"/>
+      <c r="B5" s="40"/>
+      <c r="C5" s="40"/>
+      <c r="D5" s="40"/>
+      <c r="E5" s="40"/>
+      <c r="F5" s="40"/>
+      <c r="G5" s="40"/>
+      <c r="H5" s="40"/>
+      <c r="I5" s="40"/>
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B6" s="39"/>
-      <c r="C6" s="39"/>
-      <c r="D6" s="39"/>
-      <c r="E6" s="39"/>
-      <c r="F6" s="39"/>
-      <c r="G6" s="39"/>
-      <c r="H6" s="39"/>
-      <c r="I6" s="39"/>
+      <c r="B6" s="40"/>
+      <c r="C6" s="40"/>
+      <c r="D6" s="40"/>
+      <c r="E6" s="40"/>
+      <c r="F6" s="40"/>
+      <c r="G6" s="40"/>
+      <c r="H6" s="40"/>
+      <c r="I6" s="40"/>
     </row>
     <row r="7" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B7" s="39"/>
-      <c r="C7" s="39"/>
-      <c r="D7" s="39"/>
-      <c r="E7" s="39"/>
-      <c r="F7" s="39"/>
-      <c r="G7" s="39"/>
-      <c r="H7" s="39"/>
-      <c r="I7" s="39"/>
+      <c r="B7" s="40"/>
+      <c r="C7" s="40"/>
+      <c r="D7" s="40"/>
+      <c r="E7" s="40"/>
+      <c r="F7" s="40"/>
+      <c r="G7" s="40"/>
+      <c r="H7" s="40"/>
+      <c r="I7" s="40"/>
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B8" s="39"/>
-      <c r="C8" s="39"/>
-      <c r="D8" s="39"/>
-      <c r="E8" s="39"/>
-      <c r="F8" s="39"/>
-      <c r="G8" s="39"/>
-      <c r="H8" s="39"/>
-      <c r="I8" s="39"/>
+      <c r="B8" s="40"/>
+      <c r="C8" s="40"/>
+      <c r="D8" s="40"/>
+      <c r="E8" s="40"/>
+      <c r="F8" s="40"/>
+      <c r="G8" s="40"/>
+      <c r="H8" s="40"/>
+      <c r="I8" s="40"/>
     </row>
     <row r="9" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B9" s="2"/>
@@ -15332,60 +15336,60 @@
       <c r="H1" s="3"/>
     </row>
     <row r="2" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="38" t="s">
+      <c r="B2" s="39" t="s">
         <v>100</v>
       </c>
-      <c r="C2" s="39"/>
-      <c r="D2" s="39"/>
-      <c r="E2" s="39"/>
-      <c r="F2" s="39"/>
-      <c r="G2" s="39"/>
-      <c r="H2" s="39"/>
+      <c r="C2" s="40"/>
+      <c r="D2" s="40"/>
+      <c r="E2" s="40"/>
+      <c r="F2" s="40"/>
+      <c r="G2" s="40"/>
+      <c r="H2" s="40"/>
     </row>
     <row r="3" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B3" s="39"/>
-      <c r="C3" s="39"/>
-      <c r="D3" s="39"/>
-      <c r="E3" s="39"/>
-      <c r="F3" s="39"/>
-      <c r="G3" s="39"/>
-      <c r="H3" s="39"/>
+      <c r="B3" s="40"/>
+      <c r="C3" s="40"/>
+      <c r="D3" s="40"/>
+      <c r="E3" s="40"/>
+      <c r="F3" s="40"/>
+      <c r="G3" s="40"/>
+      <c r="H3" s="40"/>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B4" s="39"/>
-      <c r="C4" s="39"/>
-      <c r="D4" s="39"/>
-      <c r="E4" s="39"/>
-      <c r="F4" s="39"/>
-      <c r="G4" s="39"/>
-      <c r="H4" s="39"/>
+      <c r="B4" s="40"/>
+      <c r="C4" s="40"/>
+      <c r="D4" s="40"/>
+      <c r="E4" s="40"/>
+      <c r="F4" s="40"/>
+      <c r="G4" s="40"/>
+      <c r="H4" s="40"/>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B5" s="39"/>
-      <c r="C5" s="39"/>
-      <c r="D5" s="39"/>
-      <c r="E5" s="39"/>
-      <c r="F5" s="39"/>
-      <c r="G5" s="39"/>
-      <c r="H5" s="39"/>
+      <c r="B5" s="40"/>
+      <c r="C5" s="40"/>
+      <c r="D5" s="40"/>
+      <c r="E5" s="40"/>
+      <c r="F5" s="40"/>
+      <c r="G5" s="40"/>
+      <c r="H5" s="40"/>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B6" s="39"/>
-      <c r="C6" s="39"/>
-      <c r="D6" s="39"/>
-      <c r="E6" s="39"/>
-      <c r="F6" s="39"/>
-      <c r="G6" s="39"/>
-      <c r="H6" s="39"/>
+      <c r="B6" s="40"/>
+      <c r="C6" s="40"/>
+      <c r="D6" s="40"/>
+      <c r="E6" s="40"/>
+      <c r="F6" s="40"/>
+      <c r="G6" s="40"/>
+      <c r="H6" s="40"/>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B7" s="39"/>
-      <c r="C7" s="39"/>
-      <c r="D7" s="39"/>
-      <c r="E7" s="39"/>
-      <c r="F7" s="39"/>
-      <c r="G7" s="39"/>
-      <c r="H7" s="39"/>
+      <c r="B7" s="40"/>
+      <c r="C7" s="40"/>
+      <c r="D7" s="40"/>
+      <c r="E7" s="40"/>
+      <c r="F7" s="40"/>
+      <c r="G7" s="40"/>
+      <c r="H7" s="40"/>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B8" s="3"/>

</xml_diff>